<commit_message>
Updated maths data structure to closer match key stage levels and lessons structure
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -363,14 +363,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -686,7 +679,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,7 +1459,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add how to play screen with new icons Stop spamming of setting data in test builds
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="158">
   <si>
     <t>Key</t>
   </si>
@@ -296,13 +296,205 @@
   </si>
   <si>
     <t>Connecting</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_OBSTACLE_TITLE</t>
+  </si>
+  <si>
+    <t>Obstacle version</t>
+  </si>
+  <si>
+    <t>Versión obstáculo</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_OBSTACLE_DESCRIPTION_A</t>
+  </si>
+  <si>
+    <t>Player B and C must help player A reach the finish point whilst avoiding obstacles.</t>
+  </si>
+  <si>
+    <t>Los jugadores B y C deben ayudar al jugador A a llegar a la meta salvando los obstáculos</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_OBSTACLE_DESCRIPTION_B</t>
+  </si>
+  <si>
+    <t>At end of each round player A can select upgrades for the other two players.</t>
+  </si>
+  <si>
+    <t>Al final de cada ronda el jugador A puede seleccionar mejoras para los otros dos jugadores</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_OBSTACLE_DESCRIPTION_C</t>
+  </si>
+  <si>
+    <t>Players swap places after each round.</t>
+  </si>
+  <si>
+    <t>Los jugadores se intercambian de posición en cada ronda</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_MATHS_TITLE</t>
+  </si>
+  <si>
+    <t>Maths version</t>
+  </si>
+  <si>
+    <t>Versión de matemáticas</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_MATHS_DESCRIPTION_A</t>
+  </si>
+  <si>
+    <t>Players B and C must help player A reach the finish point by guiding the raft through the correct calculations.</t>
+  </si>
+  <si>
+    <t>Los jugadores B y C deben ayudar al jugador A a llegar a la meta guiando la balsa hacia el resultado correcto</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_MATHS_DESCRIPTION_B</t>
+  </si>
+  <si>
+    <t>UI_INSTRUCTION_MATHS_DESCRIPTION_C</t>
+  </si>
+  <si>
+    <t>PlushyPaddles Numeracy challenges 3 players to work together, solving mathematical equations through effective communication and cooperation.</t>
+  </si>
+  <si>
+    <t>Pushy Paddles Numeracy reta a tres jugadores a trabajar juntos resolviendo problemas matemáticos a través de la comunicación y la cooperación</t>
+  </si>
+  <si>
+    <t>Conectar</t>
+  </si>
+  <si>
+    <t>Iniciar Servidor</t>
+  </si>
+  <si>
+    <t>Salir del juego</t>
+  </si>
+  <si>
+    <t>Salir del menú</t>
+  </si>
+  <si>
+    <t>Continuar</t>
+  </si>
+  <si>
+    <t>Menú</t>
+  </si>
+  <si>
+    <t>Jugar</t>
+  </si>
+  <si>
+    <t>Jugar otra vez</t>
+  </si>
+  <si>
+    <t>Pausar</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>Siguiente</t>
+  </si>
+  <si>
+    <t>Seleccionar</t>
+  </si>
+  <si>
+    <t>Cancelar</t>
+  </si>
+  <si>
+    <t>Menú principal</t>
+  </si>
+  <si>
+    <t>Dirección IP</t>
+  </si>
+  <si>
+    <t>Puerto</t>
+  </si>
+  <si>
+    <t>Cargando</t>
+  </si>
+  <si>
+    <t>Conectando</t>
+  </si>
+  <si>
+    <t>Fin del juego</t>
+  </si>
+  <si>
+    <t>Tiempo agotado</t>
+  </si>
+  <si>
+    <t>Rondas completadas</t>
+  </si>
+  <si>
+    <t>Nivel completado - Distribuir recompensas</t>
+  </si>
+  <si>
+    <t>Aumentar velocidad</t>
+  </si>
+  <si>
+    <t>Sin recompensa</t>
+  </si>
+  <si>
+    <t>Invertir controles</t>
+  </si>
+  <si>
+    <t>Propulsión</t>
+  </si>
+  <si>
+    <t>Más control de la plataforma</t>
+  </si>
+  <si>
+    <t>Selecciona un personaje</t>
+  </si>
+  <si>
+    <t>Tu ganas</t>
+  </si>
+  <si>
+    <t>Inténtalo de nuevo</t>
+  </si>
+  <si>
+    <t>Trabajad juntos para dirigiros del puente al cofre</t>
+  </si>
+  <si>
+    <t>Partida</t>
+  </si>
+  <si>
+    <t>Jugador</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Juego en pausa</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Esperando a otros jugadores...</t>
+  </si>
+  <si>
+    <t>Partidas completadas</t>
+  </si>
+  <si>
+    <t>Partida: {0}</t>
+  </si>
+  <si>
+    <t>Jugador: {0}</t>
+  </si>
+  <si>
+    <t>Objetivo: {0}</t>
+  </si>
+  <si>
+    <t>Total actual: {0}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,16 +510,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -335,11 +551,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -359,11 +590,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEA3A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEA3A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -676,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,7 +970,7 @@
     <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,757 +987,893 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C28" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C31" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C33" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C34" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C41" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C43" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C44" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="C45" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A46:XFD1048576 A3:C45 E3:XFD45 A2:B2 F2:XFD2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add victory game over screen Track player sharing based on if they give the reward to themself or not
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="212">
   <si>
     <t>Key</t>
   </si>
@@ -638,6 +638,18 @@
   </si>
   <si>
     <t>Το παιγνίδι Αριθμητικής Plushy Paddles, δημιουργεί για τους τρεις παίκτες την πρόκληση να συνεργαστούν και να επικοινωνήσουν αποτελεσματικά για την επίλυση μαθηματικών εξισώσεων.</t>
+  </si>
+  <si>
+    <t>UI_END_LESSON_COMPLETE</t>
+  </si>
+  <si>
+    <t>Lesson Complete</t>
+  </si>
+  <si>
+    <t>UI_END_TIME_TAKEN</t>
+  </si>
+  <si>
+    <t>Time Taken</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="H34:I34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1450,550 +1462,584 @@
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>29</v>
+        <v>209</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>131</v>
+      <c r="D22" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>48</v>
+        <v>210</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>173</v>
+        <v>5</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>133</v>
+      <c r="D24" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>175</v>
+        <v>132</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>137</v>
+      <c r="D28" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>179</v>
+        <v>36</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>181</v>
+      <c r="D29" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>138</v>
+      <c r="D30" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>183</v>
+      <c r="D31" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>186</v>
+      <c r="D34" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>188</v>
+      <c r="D36" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>31</v>
+        <v>79</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>193</v>
+        <v>146</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>195</v>
+        <v>148</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="10" t="s">
+      <c r="C47" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B48" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="10" t="s">
+      <c r="C48" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+    <row r="49" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="C49" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+    <row r="50" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="C50" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="C51" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E51" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="8" t="s">
+      <c r="C52" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
+    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="C53" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E53" s="8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+    <row r="54" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B54" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="8" t="s">
+      <c r="C54" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+    <row r="55" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="7" t="s">
+      <c r="C55" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E55" s="7" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A54:XFD1048576 F2:XFD53">
+  <conditionalFormatting sqref="A1:XFD1 A56:XFD1048576 F2:XFD55">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix rock spawning with new tilt ability was possible to complete levels without help
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -640,16 +640,16 @@
     <t>Το παιγνίδι Αριθμητικής Plushy Paddles, δημιουργεί για τους τρεις παίκτες την πρόκληση να συνεργαστούν και να επικοινωνήσουν αποτελεσματικά για την επίλυση μαθηματικών εξισώσεων.</t>
   </si>
   <si>
-    <t>UI_END_LESSON_COMPLETE</t>
-  </si>
-  <si>
-    <t>Lesson Complete</t>
-  </si>
-  <si>
     <t>UI_END_TIME_TAKEN</t>
   </si>
   <si>
     <t>Time Taken</t>
+  </si>
+  <si>
+    <t>UI_END_GAME_COMPLETE</t>
+  </si>
+  <si>
+    <t>Game Complete</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>5</v>
@@ -1479,10 +1479,10 @@
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add new collectible art to not be placeholder anymore
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="273">
   <si>
     <t>Key</t>
   </si>
@@ -812,6 +812,27 @@
   </si>
   <si>
     <t>Το παιγνίδι Αριθμητικής Pushy Paddles, δημιουργεί για τους τρεις παίκτες την πρόκληση να συνεργαστούν και να επικοινωνήσουν αποτελεσματικά για την επίλυση μαθηματικών εξισώσεων.</t>
+  </si>
+  <si>
+    <t>UI_LESSON_TITLE</t>
+  </si>
+  <si>
+    <t>FORMATTED_UI_LESSON</t>
+  </si>
+  <si>
+    <t>FORMATTED_UI_YEAR</t>
+  </si>
+  <si>
+    <t>Select A Lesson</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>Lesson {0}</t>
+  </si>
+  <si>
+    <t>Year {0}</t>
   </si>
 </sst>
 </file>
@@ -964,7 +985,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1277,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2228,9 +2263,60 @@
         <v>265</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A56:XFD1048576 F2:XFD55">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 F2:XFD55 A56:XFD1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added player choosing reward screen
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="275">
   <si>
     <t>Key</t>
   </si>
@@ -833,6 +833,12 @@
   </si>
   <si>
     <t>Year {0}</t>
+  </si>
+  <si>
+    <t>FORMATTED_UI_REWARDS_PLAYER_CHOOSING</t>
+  </si>
+  <si>
+    <t>{0} is choosing rewards</t>
   </si>
 </sst>
 </file>
@@ -985,21 +991,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1312,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:E58"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2314,9 +2306,26 @@
         <v>270</v>
       </c>
     </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 F2:XFD55 A56:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added changing roles ui to make it clearer
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="111" windowWidth="14811" windowHeight="8014"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="277">
   <si>
     <t>Key</t>
   </si>
@@ -839,6 +839,12 @@
   </si>
   <si>
     <t>{0} is choosing rewards</t>
+  </si>
+  <si>
+    <t>UI_GAME_CHANGING_ROLES</t>
+  </si>
+  <si>
+    <t>Changing Roles</t>
   </si>
 </sst>
 </file>
@@ -1304,23 +1310,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="43.6328125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="43.7265625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="43.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="43.54296875" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="42.53515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.61328125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="43.69140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.61328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="43.53515625" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="8.69140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>77</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1507,7 +1513,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>49</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>50</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>51</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>82</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>88</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>89</v>
       </c>
@@ -1660,7 +1666,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>205</v>
       </c>
@@ -1694,7 +1700,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>203</v>
       </c>
@@ -1711,7 +1717,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
@@ -1728,7 +1734,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>47</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>31</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>33</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>36</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>41</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>48</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
@@ -1881,7 +1887,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>58</v>
       </c>
@@ -1898,7 +1904,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>59</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>62</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>65</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>66</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>67</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>74</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>78</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>84</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>64</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>68</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>69</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>80</v>
       </c>
@@ -2102,7 +2108,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>86</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>92</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="23.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>94</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="23.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>97</v>
       </c>
@@ -2170,7 +2176,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>100</v>
       </c>
@@ -2187,7 +2193,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>103</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="35.15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>106</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="23.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>108</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="46.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>109</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>266</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>267</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>268</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>273</v>
       </c>
@@ -2320,6 +2326,23 @@
         <v>270</v>
       </c>
       <c r="E59" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" s="13" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update localizations Update dlls Update streaming assets to use port 49768
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="291">
   <si>
     <t>Key</t>
   </si>
@@ -823,9 +823,6 @@
     <t>Select A Lesson</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
     <t>Lesson {0}</t>
   </si>
   <si>
@@ -875,13 +872,28 @@
   </si>
   <si>
     <t>Cambiar roles</t>
+  </si>
+  <si>
+    <t>Επιλογή Μαθήματος</t>
+  </si>
+  <si>
+    <t>Μάθημα {0}</t>
+  </si>
+  <si>
+    <t>Τάξη {0}</t>
+  </si>
+  <si>
+    <t>Ποιος διαλέγει ανταμοιβές: {0}</t>
+  </si>
+  <si>
+    <t>Αλλαγή Ρόλων</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,6 +964,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -994,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1039,6 +1057,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1361,7 +1382,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1379,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2317,13 +2338,13 @@
         <v>268</v>
       </c>
       <c r="C56" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>269</v>
+      <c r="E56" s="16" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2331,16 +2352,16 @@
         <v>266</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C57" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>269</v>
+      <c r="E57" s="16" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2348,54 +2369,54 @@
         <v>267</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C58" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>269</v>
+      <c r="E58" s="16" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B59" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="B59" s="13" t="s">
-        <v>273</v>
-      </c>
       <c r="C59" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>269</v>
+      <c r="E59" s="16" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B60" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="B60" s="13" t="s">
-        <v>275</v>
-      </c>
       <c r="C60" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>269</v>
+      <c r="E60" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 F2:XFD55 A61:XFD1048576 A56:B60 E56:XFD60">
+  <conditionalFormatting sqref="A1:XFD1 A61:XFD1048576 A56:B60 F2:XFD60">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add quality settings to UI so it can be controlled from a device
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="296">
   <si>
     <t>Key</t>
   </si>
@@ -887,6 +887,21 @@
   </si>
   <si>
     <t>Αλλαγή Ρόλων</t>
+  </si>
+  <si>
+    <t>UI_QUALITY</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Qualità</t>
+  </si>
+  <si>
+    <t>Ποιότητα</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1062,6 +1077,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1379,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2415,8 +2431,25 @@
         <v>290</v>
       </c>
     </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A61:XFD1048576 A56:B60 F2:XFD60">
+  <conditionalFormatting sqref="A1:XFD1 A62:XFD1048576 A56:B61 F2:XFD61">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Descriptions for levels added to the spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="442">
   <si>
     <t>Key</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Selecciona un personaje</t>
   </si>
   <si>
-    <t>Tu ganas</t>
-  </si>
-  <si>
     <t>Inténtalo de nuevo</t>
   </si>
   <si>
@@ -802,9 +799,6 @@
     <t>I giocatori B e C devono aiutare il giocatore A a raggiungere il punto finale guidando la zattera con i giusti calcoli</t>
   </si>
   <si>
-    <t>Los jugadores B y C deben ayudar al jugador A a llegar a la meta guiando la lancha hacia el resultado correcto</t>
-  </si>
-  <si>
     <t>La sfida dei tre giocatori nel remare con forza grazie a calcoli matematici, risoluzione di equazioni sviluppate attraverso una vera cooperazione ed una concreta comunicazione</t>
   </si>
   <si>
@@ -902,13 +896,457 @@
   </si>
   <si>
     <t>Ποιότητα</t>
+  </si>
+  <si>
+    <t>Los jugadores B y C deben ayudar al jugador A a llegar a la meta guiando la lancha mediante los cálculos correctos</t>
+  </si>
+  <si>
+    <t>Conseguido</t>
+  </si>
+  <si>
+    <t>Bien hecho</t>
+  </si>
+  <si>
+    <t>LESSON_1</t>
+  </si>
+  <si>
+    <t>add two one-digit numbers to 18</t>
+  </si>
+  <si>
+    <t>Sumar dos números de un dígito a 18</t>
+  </si>
+  <si>
+    <t>LESSON_2</t>
+  </si>
+  <si>
+    <t>add a one and a two-digit numbers to 19</t>
+  </si>
+  <si>
+    <t>Sumar un número de un dígito y un número de dos dígitos a 19</t>
+  </si>
+  <si>
+    <t>LESSON_3</t>
+  </si>
+  <si>
+    <t>subtract one-digit numbers to zero</t>
+  </si>
+  <si>
+    <t>Restar números de un dígito a cero</t>
+  </si>
+  <si>
+    <t>LESSON_4</t>
+  </si>
+  <si>
+    <t>subtract one and two-digit numbers to zero</t>
+  </si>
+  <si>
+    <t>Restar números de un dígito y de dos dígitos a cero</t>
+  </si>
+  <si>
+    <t>LESSON_5</t>
+  </si>
+  <si>
+    <t>add and subtract one-digit numbers to 18</t>
+  </si>
+  <si>
+    <t>Sumar y restar números de un dígito a 18</t>
+  </si>
+  <si>
+    <t>LESSON_6</t>
+  </si>
+  <si>
+    <t>add and subtract one and two-digit numbers to 20 including zero</t>
+  </si>
+  <si>
+    <t>Sumar y restar números de un dígito y de dos dígitos a 20 incluyendo el cero</t>
+  </si>
+  <si>
+    <t>LESSON_7</t>
+  </si>
+  <si>
+    <t>add two-digit numbers and ones</t>
+  </si>
+  <si>
+    <t>Sumar números de dos dígitos y unidades</t>
+  </si>
+  <si>
+    <t>LESSON_8</t>
+  </si>
+  <si>
+    <t>add two-digit numbers and tens</t>
+  </si>
+  <si>
+    <t>Sumar números de dos dígitos y decenas</t>
+  </si>
+  <si>
+    <t>LESSON_9</t>
+  </si>
+  <si>
+    <t>add two two-digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar dos números de dos dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_10</t>
+  </si>
+  <si>
+    <t>add three one-digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar tres números de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_11</t>
+  </si>
+  <si>
+    <t>subtract a two-digit number and ones</t>
+  </si>
+  <si>
+    <t>Restar un número de dos dígitos y unidades</t>
+  </si>
+  <si>
+    <t>LESSON_12</t>
+  </si>
+  <si>
+    <t>subtract a two-digit number and tens</t>
+  </si>
+  <si>
+    <t>Restar un número de dos dígitos y decenas</t>
+  </si>
+  <si>
+    <t>LESSON_13</t>
+  </si>
+  <si>
+    <t>subtract two two-digit numbers to zero</t>
+  </si>
+  <si>
+    <t>Restar dos números de dos dígitos a cero</t>
+  </si>
+  <si>
+    <t>LESSON_14</t>
+  </si>
+  <si>
+    <t>subtract three one-digit numbers to zero</t>
+  </si>
+  <si>
+    <t>Restar tres números de un dígito a cero</t>
+  </si>
+  <si>
+    <t>LESSON_15</t>
+  </si>
+  <si>
+    <t>add and subtract three two-digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar y restar tres números de dos dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_16</t>
+  </si>
+  <si>
+    <t>multiply 2 times table to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 2 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_17</t>
+  </si>
+  <si>
+    <t>multiply 10 times table to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 10 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_18</t>
+  </si>
+  <si>
+    <t>multiply 5 times table to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 5 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_19</t>
+  </si>
+  <si>
+    <t>multiply 2,5,10 with two-digit numbers</t>
+  </si>
+  <si>
+    <t>Multiplicar 2, 5, 10 con números de dos dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_20</t>
+  </si>
+  <si>
+    <t>add a three-digit number and ones</t>
+  </si>
+  <si>
+    <t>Sumar un número de tres dígitos y unidades</t>
+  </si>
+  <si>
+    <t>LESSON_21</t>
+  </si>
+  <si>
+    <t>add a three-digit number and tens</t>
+  </si>
+  <si>
+    <t>Sumar un número de tres dígitos y decenas</t>
+  </si>
+  <si>
+    <t>LESSON_22</t>
+  </si>
+  <si>
+    <t>add a three-digit numbers and hundreds</t>
+  </si>
+  <si>
+    <t>Sumar un número de tres dígitos y centenas</t>
+  </si>
+  <si>
+    <t>LESSON_23</t>
+  </si>
+  <si>
+    <t>subtract a three-digit number and ones</t>
+  </si>
+  <si>
+    <t>Restar un número de tres dígitos y unidades</t>
+  </si>
+  <si>
+    <t>LESSON_24</t>
+  </si>
+  <si>
+    <t>subtract a three-digit number and tens</t>
+  </si>
+  <si>
+    <t>Restar un número de tres dígitos y decenas</t>
+  </si>
+  <si>
+    <t>LESSON_25</t>
+  </si>
+  <si>
+    <t>subtract a three-digit numbers and hundreds</t>
+  </si>
+  <si>
+    <t>Restar un número de tres dígitos y centenas</t>
+  </si>
+  <si>
+    <t>LESSON_26</t>
+  </si>
+  <si>
+    <t>add and subtract a three-digit number and ones</t>
+  </si>
+  <si>
+    <t>Sumar y restar un número de tres dígitos y unidades</t>
+  </si>
+  <si>
+    <t>LESSON_27</t>
+  </si>
+  <si>
+    <t>add and subtract a three-digit number and tens</t>
+  </si>
+  <si>
+    <t>Sumar y restar un número de tres dígitos y decenas</t>
+  </si>
+  <si>
+    <t>LESSON_28</t>
+  </si>
+  <si>
+    <t>add and subtract a three-digit numbers and hundreds</t>
+  </si>
+  <si>
+    <t>Sumar y restar un número de tres dígitos y centenas</t>
+  </si>
+  <si>
+    <t>LESSON_29</t>
+  </si>
+  <si>
+    <t>multiply 3 times table to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 3 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_30</t>
+  </si>
+  <si>
+    <t>multipyh 4 times table up to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 4 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_31</t>
+  </si>
+  <si>
+    <t>divide by 10 and 100</t>
+  </si>
+  <si>
+    <t>Dividir por 10 y 100</t>
+  </si>
+  <si>
+    <t>LESSON_32</t>
+  </si>
+  <si>
+    <t>multiply 8 times table to 12</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 8 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_33</t>
+  </si>
+  <si>
+    <t>add and subtract two three-digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar y restar dos números de tres dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_34</t>
+  </si>
+  <si>
+    <t>add four digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar números de cuatro dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_35</t>
+  </si>
+  <si>
+    <t>subtract four digit numbers</t>
+  </si>
+  <si>
+    <t>Restar números de cuatro dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_36</t>
+  </si>
+  <si>
+    <t>add and subtract four digit numbers</t>
+  </si>
+  <si>
+    <t>Sumar y restar números de cuatro dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_37</t>
+  </si>
+  <si>
+    <t>multiply 12 x 12 times table</t>
+  </si>
+  <si>
+    <t>Multiplicar la tabla del 12 hasta el 12</t>
+  </si>
+  <si>
+    <t>LESSON_38</t>
+  </si>
+  <si>
+    <t>multiply two-digit number by one-digit number</t>
+  </si>
+  <si>
+    <t>Multiplicar un número de dos dígitos por un número de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_39</t>
+  </si>
+  <si>
+    <t>multiply three-digit number by one-digit number</t>
+  </si>
+  <si>
+    <t>Multiplicar un número de tres dígitos por un número de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_40</t>
+  </si>
+  <si>
+    <t>divide two-digit number by one-digit number</t>
+  </si>
+  <si>
+    <t>Dividir un número de dos dígitos entre un número de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_41</t>
+  </si>
+  <si>
+    <t>divide three-digit number by one-digit number</t>
+  </si>
+  <si>
+    <t>Dividir un número de tres dígitos entre un número de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_42</t>
+  </si>
+  <si>
+    <t>multiply up to 4 digits by one-digit</t>
+  </si>
+  <si>
+    <t>Multiplicar 4 dígitos por un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_43</t>
+  </si>
+  <si>
+    <t>recognise square numbers and notation</t>
+  </si>
+  <si>
+    <t>Reconocer números cuadrados y su notación</t>
+  </si>
+  <si>
+    <t>LESSON_44</t>
+  </si>
+  <si>
+    <t>recognise cube numbers and notation</t>
+  </si>
+  <si>
+    <t>Reconocer números cúbicos y su notación</t>
+  </si>
+  <si>
+    <t>LESSON_45</t>
+  </si>
+  <si>
+    <t>divide numbers up to 4 digits by a one-digit number</t>
+  </si>
+  <si>
+    <t>Dividir números de más de 4 dígitos entre un número de un dígito</t>
+  </si>
+  <si>
+    <t>LESSON_46</t>
+  </si>
+  <si>
+    <t>solve one operations (+, –, ÷, ×) up to 4 digits</t>
+  </si>
+  <si>
+    <t>Resolver una operación (+, –, ÷, ×) de más de 4 dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_47</t>
+  </si>
+  <si>
+    <t>solve two operation up to 4 digits</t>
+  </si>
+  <si>
+    <t>Resolver dos operaciones de más de 4 dígitos</t>
+  </si>
+  <si>
+    <t>LESSON_48</t>
+  </si>
+  <si>
+    <t>solve three operations up to 4 digits</t>
+  </si>
+  <si>
+    <t>Resolver tres operaciones de más de 4 dígitos</t>
+  </si>
+  <si>
+    <t>XXXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,8 +1423,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -996,6 +1440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,7 +1477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1078,6 +1528,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,10 +1861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1453,13 +1919,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1470,13 +1936,13 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1487,13 +1953,13 @@
         <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1504,13 +1970,13 @@
         <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1521,13 +1987,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1538,13 +2004,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>114</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1555,13 +2021,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>115</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1572,13 +2038,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1589,13 +2055,13 @@
         <v>17</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>117</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1606,13 +2072,13 @@
         <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1623,13 +2089,13 @@
         <v>52</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1640,13 +2106,13 @@
         <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>120</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1657,13 +2123,13 @@
         <v>82</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1674,13 +2140,13 @@
         <v>75</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>122</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1691,13 +2157,13 @@
         <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>123</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1708,13 +2174,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>124</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1725,13 +2191,13 @@
         <v>89</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>125</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1742,13 +2208,13 @@
         <v>90</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>126</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,47 +2225,47 @@
         <v>26</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="C22" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="12" t="s">
         <v>226</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>203</v>
-      </c>
       <c r="C23" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1810,13 +2276,13 @@
         <v>27</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1827,13 +2293,13 @@
         <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>129</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1844,13 +2310,13 @@
         <v>31</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>130</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1861,13 +2327,13 @@
         <v>36</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>131</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1878,13 +2344,13 @@
         <v>37</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1895,13 +2361,13 @@
         <v>38</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>133</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1912,13 +2378,13 @@
         <v>39</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>134</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1926,16 +2392,16 @@
         <v>40</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1946,13 +2412,13 @@
         <v>54</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>135</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1963,13 +2429,13 @@
         <v>56</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>56</v>
+        <v>241</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>295</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1980,13 +2446,13 @@
         <v>60</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>136</v>
+        <v>242</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1997,13 +2463,13 @@
         <v>59</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2014,13 +2480,13 @@
         <v>62</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2031,13 +2497,13 @@
         <v>69</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2048,13 +2514,13 @@
         <v>70</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2068,10 +2534,10 @@
         <v>13</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2082,13 +2548,13 @@
         <v>74</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2099,13 +2565,13 @@
         <v>78</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2116,13 +2582,13 @@
         <v>84</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2133,13 +2599,13 @@
         <v>29</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2150,13 +2616,13 @@
         <v>71</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2167,13 +2633,13 @@
         <v>72</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2184,13 +2650,13 @@
         <v>80</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2201,13 +2667,13 @@
         <v>86</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2218,13 +2684,13 @@
         <v>92</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D48" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2235,13 +2701,13 @@
         <v>94</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2249,16 +2715,16 @@
         <v>96</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2269,13 +2735,13 @@
         <v>100</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2286,13 +2752,13 @@
         <v>103</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>104</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
@@ -2303,13 +2769,13 @@
         <v>106</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>294</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2320,13 +2786,13 @@
         <v>97</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2334,122 +2800,938 @@
         <v>108</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E60" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="C61" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="D61" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="B61" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="D61" s="17" t="s">
+      <c r="E61" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="E61" s="17" t="s">
-        <v>295</v>
+    </row>
+    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D85" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D90" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="E95" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="E97" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="20" t="s">
+        <v>405</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="E100" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="E101" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D103" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D104" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="E104" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D105" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="E105" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="E106" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D107" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E107" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D108" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D109" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="E109" s="22" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A62:XFD1048576 A56:B61 F2:XFD61">
+  <conditionalFormatting sqref="A1:XFD1 A110:XFD1048576 A56:B61 F2:XFD109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add increase and decrease tide powerups so there are more for sindle player
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="446">
   <si>
     <t>Key</t>
   </si>
@@ -1340,6 +1340,18 @@
   </si>
   <si>
     <t>XXXX</t>
+  </si>
+  <si>
+    <t>UI_REWARDS_DECREASE_TIDE</t>
+  </si>
+  <si>
+    <t>UI_REWARDS_INCREASE_TIDE</t>
+  </si>
+  <si>
+    <t>Water Speed Increased</t>
+  </si>
+  <si>
+    <t>Water Speed Decreased</t>
   </si>
 </sst>
 </file>
@@ -1861,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2406,577 +2418,577 @@
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>47</v>
+        <v>442</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>54</v>
+        <v>445</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>135</v>
+        <v>441</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>441</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>176</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>55</v>
+        <v>443</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>56</v>
+        <v>444</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>295</v>
+        <v>441</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>441</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>177</v>
+        <v>441</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>296</v>
+        <v>240</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>136</v>
+        <v>241</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>295</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>137</v>
+        <v>242</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>139</v>
+        <v>244</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>13</v>
+        <v>245</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B49" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E49" s="12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+    <row r="51" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B51" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+    <row r="52" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C54" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D54" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+    <row r="55" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D55" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
+    <row r="56" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E56" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+    <row r="57" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B57" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>280</v>
+        <v>267</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>276</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B62" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E62" s="16" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B63" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D63" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E63" s="17" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>299</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="20" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E64" s="22" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="20" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E65" s="22" t="s">
         <v>441</v>
@@ -2984,33 +2996,33 @@
     </row>
     <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="20" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E66" s="22" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="20" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C67" s="22" t="s">
         <v>441</v>
       </c>
-      <c r="D67" s="23" t="s">
-        <v>314</v>
+      <c r="D67" s="22" t="s">
+        <v>308</v>
       </c>
       <c r="E67" s="22" t="s">
         <v>441</v>
@@ -3018,33 +3030,33 @@
     </row>
     <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="20" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E68" s="22" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="20" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>441</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>320</v>
+      <c r="D69" s="23" t="s">
+        <v>314</v>
       </c>
       <c r="E69" s="22" t="s">
         <v>441</v>
@@ -3052,16 +3064,16 @@
     </row>
     <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="20" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>441</v>
@@ -3069,16 +3081,16 @@
     </row>
     <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="20" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E71" s="22" t="s">
         <v>441</v>
@@ -3086,16 +3098,16 @@
     </row>
     <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="20" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C72" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E72" s="22" t="s">
         <v>441</v>
@@ -3103,16 +3115,16 @@
     </row>
     <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="20" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C73" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E73" s="22" t="s">
         <v>441</v>
@@ -3120,16 +3132,16 @@
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="20" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C74" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E74" s="22" t="s">
         <v>441</v>
@@ -3137,16 +3149,16 @@
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="20" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C75" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E75" s="22" t="s">
         <v>441</v>
@@ -3154,16 +3166,16 @@
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="20" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E76" s="22" t="s">
         <v>441</v>
@@ -3171,16 +3183,16 @@
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="20" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C77" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E77" s="22" t="s">
         <v>441</v>
@@ -3188,16 +3200,16 @@
     </row>
     <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="20" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C78" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E78" s="22" t="s">
         <v>441</v>
@@ -3205,16 +3217,16 @@
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="20" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C79" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E79" s="22" t="s">
         <v>441</v>
@@ -3222,16 +3234,16 @@
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="20" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C80" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E80" s="22" t="s">
         <v>441</v>
@@ -3239,16 +3251,16 @@
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="20" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C81" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E81" s="22" t="s">
         <v>441</v>
@@ -3256,16 +3268,16 @@
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="20" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C82" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E82" s="22" t="s">
         <v>441</v>
@@ -3273,16 +3285,16 @@
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="20" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C83" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E83" s="22" t="s">
         <v>441</v>
@@ -3290,16 +3302,16 @@
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="20" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C84" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E84" s="22" t="s">
         <v>441</v>
@@ -3307,16 +3319,16 @@
     </row>
     <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="20" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C85" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E85" s="22" t="s">
         <v>441</v>
@@ -3324,16 +3336,16 @@
     </row>
     <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="20" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E86" s="22" t="s">
         <v>441</v>
@@ -3341,16 +3353,16 @@
     </row>
     <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="20" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C87" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E87" s="22" t="s">
         <v>441</v>
@@ -3358,33 +3370,33 @@
     </row>
     <row r="88" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="20" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C88" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E88" s="22" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="20" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C89" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E89" s="22" t="s">
         <v>441</v>
@@ -3392,33 +3404,33 @@
     </row>
     <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="20" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C90" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="E90" s="22" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="20" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E91" s="22" t="s">
         <v>441</v>
@@ -3426,16 +3438,16 @@
     </row>
     <row r="92" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="20" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C92" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E92" s="22" t="s">
         <v>441</v>
@@ -3443,16 +3455,16 @@
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="20" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C93" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="E93" s="22" t="s">
         <v>441</v>
@@ -3460,16 +3472,16 @@
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="20" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C94" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E94" s="22" t="s">
         <v>441</v>
@@ -3477,16 +3489,16 @@
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="20" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C95" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E95" s="22" t="s">
         <v>441</v>
@@ -3494,16 +3506,16 @@
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="20" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C96" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E96" s="22" t="s">
         <v>441</v>
@@ -3511,16 +3523,16 @@
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="20" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C97" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D97" s="22" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E97" s="22" t="s">
         <v>441</v>
@@ -3528,50 +3540,50 @@
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="B98" s="21" t="s">
+      <c r="B100" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="C98" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D98" s="22" t="s">
+      <c r="C100" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D100" s="22" t="s">
         <v>407</v>
-      </c>
-      <c r="E98" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="20" t="s">
-        <v>408</v>
-      </c>
-      <c r="B99" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D99" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="E99" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="20" t="s">
-        <v>411</v>
-      </c>
-      <c r="B100" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D100" s="22" t="s">
-        <v>413</v>
       </c>
       <c r="E100" s="22" t="s">
         <v>441</v>
@@ -3579,16 +3591,16 @@
     </row>
     <row r="101" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="20" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C101" s="22" t="s">
         <v>441</v>
       </c>
       <c r="D101" s="22" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="E101" s="22" t="s">
         <v>441</v>
@@ -3596,50 +3608,50 @@
     </row>
     <row r="102" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D103" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="B102" s="21" t="s">
+      <c r="B104" s="21" t="s">
         <v>418</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D102" s="22" t="s">
+      <c r="C104" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D104" s="22" t="s">
         <v>419</v>
-      </c>
-      <c r="E102" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="B103" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D103" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="E103" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="B104" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D104" s="22" t="s">
-        <v>425</v>
       </c>
       <c r="E104" s="22" t="s">
         <v>441</v>
@@ -3647,91 +3659,125 @@
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D105" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E105" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="E106" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="B107" s="21" t="s">
         <v>427</v>
       </c>
-      <c r="C105" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D105" s="22" t="s">
+      <c r="C107" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D107" s="22" t="s">
         <v>428</v>
       </c>
-      <c r="E105" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="20" t="s">
+      <c r="E107" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="B106" s="21" t="s">
+      <c r="B108" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="C106" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D106" s="22" t="s">
+      <c r="C108" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D108" s="22" t="s">
         <v>431</v>
       </c>
-      <c r="E106" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="20" t="s">
+      <c r="E108" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="B107" s="21" t="s">
+      <c r="B109" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="C107" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D107" s="22" t="s">
+      <c r="C109" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D109" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="E107" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="20" t="s">
+      <c r="E109" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="20" t="s">
         <v>435</v>
       </c>
-      <c r="B108" s="21" t="s">
+      <c r="B110" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="C108" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D108" s="22" t="s">
+      <c r="C110" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D110" s="22" t="s">
         <v>437</v>
       </c>
-      <c r="E108" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="20" t="s">
+      <c r="E110" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="20" t="s">
         <v>438</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B111" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="C109" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D109" s="22" t="s">
+      <c r="C111" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D111" s="22" t="s">
         <v>440</v>
       </c>
-      <c r="E109" s="22" t="s">
+      <c r="E111" s="22" t="s">
         <v>441</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A110:XFD1048576 A56:B61 F2:XFD109">
+  <conditionalFormatting sqref="A1:XFD1 A112:XFD1048576 A58:B63 F2:XFD111">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update PSL Orchestrator .dlls Add touch movement toggle for webgl improve touch movement and controls
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="451">
   <si>
     <t>Key</t>
   </si>
@@ -1352,13 +1352,28 @@
   </si>
   <si>
     <t>Water Speed Decreased</t>
+  </si>
+  <si>
+    <t>BUTTON_TOGGLE_TOUCH</t>
+  </si>
+  <si>
+    <t>Use Tap Controls</t>
+  </si>
+  <si>
+    <t>Αγγίξτε τα στοιχεία ελέγχου</t>
+  </si>
+  <si>
+    <t>Tocca Controlli</t>
+  </si>
+  <si>
+    <t>Controles táctiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1441,6 +1456,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1489,7 +1515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1554,6 +1580,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1873,13 +1903,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="42.54296875" style="3" customWidth="1"/>
     <col min="2" max="2" width="43.6328125" style="13" customWidth="1"/>
@@ -1889,7 +1919,7 @@
     <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>76</v>
       </c>
@@ -1923,7 +1953,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1940,7 +1970,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1957,7 +1987,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +2004,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -1991,7 +2021,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2008,7 +2038,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2025,7 +2055,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -2042,7 +2072,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2059,7 +2089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2076,7 +2106,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2093,7 +2123,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2110,7 +2140,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2127,7 +2157,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="7" t="s">
         <v>81</v>
       </c>
@@ -2144,1640 +2174,1657 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" thickBot="1">
       <c r="A16" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>449</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>450</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1">
+      <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="18" spans="1:5" ht="15" thickBot="1">
+      <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E18" s="12" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:5" ht="15" thickBot="1">
+      <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:5" ht="15" thickBot="1">
+      <c r="A20" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+    <row r="21" spans="1:5" ht="15" thickBot="1">
+      <c r="A21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="22" spans="1:5" ht="15" thickBot="1">
+      <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:5" ht="15" thickBot="1">
+      <c r="A23" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:5" ht="15" thickBot="1">
+      <c r="A24" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E24" s="12" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:5" ht="15" thickBot="1">
+      <c r="A25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="1:5" ht="15" thickBot="1">
+      <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E26" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:5" ht="15" thickBot="1">
+      <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:5" ht="15" thickBot="1">
+      <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:5" ht="15" thickBot="1">
+      <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E29" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="1:5" ht="15" thickBot="1">
+      <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E30" s="12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:5" ht="15" thickBot="1">
+      <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E31" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+    <row r="32" spans="1:5" ht="15" thickBot="1">
+      <c r="A32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E32" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:5" ht="15" thickBot="1">
+      <c r="A33" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B33" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="C33" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1">
+      <c r="A34" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="C34" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1">
+      <c r="A35" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+    <row r="36" spans="1:5" ht="15" thickBot="1">
+      <c r="A36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B36" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E36" s="12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:5" ht="15" thickBot="1">
+      <c r="A37" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D37" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E37" s="12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:5" ht="15" thickBot="1">
+      <c r="A38" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+    <row r="39" spans="1:5" ht="23.5" thickBot="1">
+      <c r="A39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E39" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:5" ht="15" thickBot="1">
+      <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E40" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:5" ht="15" thickBot="1">
+      <c r="A41" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E41" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:5" ht="15" thickBot="1">
+      <c r="A42" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E42" s="12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+    <row r="43" spans="1:5" ht="15" thickBot="1">
+      <c r="A43" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B43" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E43" s="12" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+    <row r="44" spans="1:5" ht="15" thickBot="1">
+      <c r="A44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E44" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:5" ht="15" thickBot="1">
+      <c r="A45" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E45" s="12" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:5" ht="15" thickBot="1">
+      <c r="A46" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E46" s="12" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:5" ht="15" thickBot="1">
+      <c r="A47" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B47" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:5" ht="15" thickBot="1">
+      <c r="A48" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E48" s="12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:5" ht="15" thickBot="1">
+      <c r="A49" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B49" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E49" s="12" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+    <row r="50" spans="1:5" ht="15" thickBot="1">
+      <c r="A50" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+    <row r="51" spans="1:5" ht="15" thickBot="1">
+      <c r="A51" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B51" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
+    <row r="52" spans="1:5" ht="23.5" thickBot="1">
+      <c r="A52" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+    <row r="53" spans="1:5" ht="23.5" thickBot="1">
+      <c r="A53" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+    <row r="54" spans="1:5" ht="15" thickBot="1">
+      <c r="A54" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C54" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
+    <row r="55" spans="1:5" ht="15" thickBot="1">
+      <c r="A55" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+    <row r="56" spans="1:5" ht="35" thickBot="1">
+      <c r="A56" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D56" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E56" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
+    <row r="57" spans="1:5" ht="23.5" thickBot="1">
+      <c r="A57" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B57" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+    <row r="58" spans="1:5" ht="46.5" thickBot="1">
+      <c r="A58" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B58" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E58" s="12" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:5" ht="15" thickBot="1">
+      <c r="A59" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C59" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D59" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E59" s="16" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="3" t="s">
+    <row r="60" spans="1:5" ht="15" thickBot="1">
+      <c r="A60" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B60" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C60" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D60" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E60" s="16" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="3" t="s">
+    <row r="61" spans="1:5" ht="15" thickBot="1">
+      <c r="A61" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B61" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C61" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D61" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E61" s="16" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="3" t="s">
+    <row r="62" spans="1:5" ht="15" thickBot="1">
+      <c r="A62" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B62" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E62" s="16" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:5" ht="15" thickBot="1">
+      <c r="A63" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B63" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D63" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E63" s="16" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="64" spans="1:5" ht="15" thickBot="1">
+      <c r="A64" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B64" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D64" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="20" t="s">
+    <row r="65" spans="1:5" ht="15" thickBot="1">
+      <c r="A65" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B65" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="C64" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D64" s="22" t="s">
+      <c r="C65" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="E64" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="20" t="s">
+      <c r="E65" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A66" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B66" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D65" s="22" t="s">
+      <c r="C66" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D66" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="E65" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="20" t="s">
+      <c r="E66" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1">
+      <c r="A67" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B67" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="C66" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D66" s="22" t="s">
+      <c r="C67" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D67" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="E66" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="20" t="s">
+      <c r="E67" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" thickBot="1">
+      <c r="A68" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B68" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="C67" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D67" s="22" t="s">
+      <c r="C68" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="E67" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="20" t="s">
+      <c r="E68" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" thickBot="1">
+      <c r="A69" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="B68" s="21" t="s">
+      <c r="B69" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D68" s="22" t="s">
+      <c r="C69" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D69" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="E68" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="20" t="s">
+      <c r="E69" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A70" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B70" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D69" s="23" t="s">
+      <c r="C70" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D70" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="E69" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="20" t="s">
+      <c r="E70" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" thickBot="1">
+      <c r="A71" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B71" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D70" s="22" t="s">
+      <c r="C71" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D71" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="E70" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="20" t="s">
+      <c r="E71" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1">
+      <c r="A72" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B72" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="C71" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D71" s="22" t="s">
+      <c r="C72" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D72" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="E71" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="20" t="s">
+      <c r="E72" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15" thickBot="1">
+      <c r="A73" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B73" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D72" s="22" t="s">
+      <c r="C73" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D73" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="E72" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="20" t="s">
+      <c r="E73" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15" thickBot="1">
+      <c r="A74" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="B73" s="21" t="s">
+      <c r="B74" s="21" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D73" s="22" t="s">
+      <c r="C74" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="20" t="s">
+      <c r="E74" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" thickBot="1">
+      <c r="A75" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="B74" s="21" t="s">
+      <c r="B75" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="C74" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D74" s="22" t="s">
+      <c r="C75" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D75" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="20" t="s">
+      <c r="E75" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" thickBot="1">
+      <c r="A76" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B76" s="21" t="s">
         <v>331</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D75" s="22" t="s">
+      <c r="C76" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D76" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="E75" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="20" t="s">
+      <c r="E76" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" thickBot="1">
+      <c r="A77" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="B76" s="21" t="s">
+      <c r="B77" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="C76" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D76" s="22" t="s">
+      <c r="C77" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="E76" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="20" t="s">
+      <c r="E77" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1">
+      <c r="A78" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B78" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="C77" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D77" s="22" t="s">
+      <c r="C78" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D78" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="20" t="s">
+      <c r="E78" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" thickBot="1">
+      <c r="A79" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="B78" s="21" t="s">
+      <c r="B79" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="C78" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D78" s="22" t="s">
+      <c r="C79" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="E78" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="20" t="s">
+      <c r="E79" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" thickBot="1">
+      <c r="A80" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B80" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="C79" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D79" s="22" t="s">
+      <c r="C80" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="20" t="s">
+      <c r="E80" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" thickBot="1">
+      <c r="A81" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="B80" s="21" t="s">
+      <c r="B81" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="C80" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D80" s="22" t="s">
+      <c r="C81" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="E80" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="20" t="s">
+      <c r="E81" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15" thickBot="1">
+      <c r="A82" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B82" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="C81" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D81" s="22" t="s">
+      <c r="C82" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D82" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="E81" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="20" t="s">
+      <c r="E82" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15" thickBot="1">
+      <c r="A83" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="B82" s="21" t="s">
+      <c r="B83" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="C82" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D82" s="22" t="s">
+      <c r="C83" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E82" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="20" t="s">
+      <c r="E83" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15" thickBot="1">
+      <c r="A84" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B84" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="C83" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D83" s="22" t="s">
+      <c r="C84" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D84" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="20" t="s">
+      <c r="E84" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" thickBot="1">
+      <c r="A85" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="B84" s="21" t="s">
+      <c r="B85" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="C84" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D84" s="22" t="s">
+      <c r="C85" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="20" t="s">
+      <c r="E85" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15" thickBot="1">
+      <c r="A86" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B86" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="C85" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D85" s="22" t="s">
+      <c r="C86" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D86" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="20" t="s">
+      <c r="E86" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15" thickBot="1">
+      <c r="A87" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="B87" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="C86" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D86" s="22" t="s">
+      <c r="C87" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="E86" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="20" t="s">
+      <c r="E87" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15" thickBot="1">
+      <c r="A88" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="B87" s="21" t="s">
+      <c r="B88" s="21" t="s">
         <v>367</v>
       </c>
-      <c r="C87" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D87" s="22" t="s">
+      <c r="C88" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D88" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="E87" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="20" t="s">
+      <c r="E88" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15" thickBot="1">
+      <c r="A89" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="B88" s="21" t="s">
+      <c r="B89" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="C88" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D88" s="22" t="s">
+      <c r="C89" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D89" s="22" t="s">
         <v>371</v>
       </c>
-      <c r="E88" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="20" t="s">
+      <c r="E89" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15" thickBot="1">
+      <c r="A90" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B90" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="C89" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D89" s="22" t="s">
+      <c r="C90" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D90" s="22" t="s">
         <v>374</v>
       </c>
-      <c r="E89" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="20" t="s">
+      <c r="E90" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" thickBot="1">
+      <c r="A91" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="B90" s="21" t="s">
+      <c r="B91" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="C90" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D90" s="22" t="s">
+      <c r="C91" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="E90" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="20" t="s">
+      <c r="E91" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A92" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="B91" s="21" t="s">
+      <c r="B92" s="21" t="s">
         <v>379</v>
       </c>
-      <c r="C91" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D91" s="22" t="s">
+      <c r="C92" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D92" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="E91" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="20" t="s">
+      <c r="E92" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" thickBot="1">
+      <c r="A93" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="B92" s="21" t="s">
+      <c r="B93" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="C92" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D92" s="22" t="s">
+      <c r="C93" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D93" s="22" t="s">
         <v>383</v>
       </c>
-      <c r="E92" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="20" t="s">
+      <c r="E93" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" thickBot="1">
+      <c r="A94" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="B93" s="21" t="s">
+      <c r="B94" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="C93" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D93" s="22" t="s">
+      <c r="C94" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D94" s="22" t="s">
         <v>386</v>
       </c>
-      <c r="E93" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="20" t="s">
+      <c r="E94" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15" thickBot="1">
+      <c r="A95" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="B94" s="21" t="s">
+      <c r="B95" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="C94" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D94" s="22" t="s">
+      <c r="C95" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D95" s="22" t="s">
         <v>389</v>
       </c>
-      <c r="E94" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="20" t="s">
+      <c r="E95" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15" thickBot="1">
+      <c r="A96" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="B95" s="21" t="s">
+      <c r="B96" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="C95" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D95" s="22" t="s">
+      <c r="C96" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D96" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="E95" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="20" t="s">
+      <c r="E96" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15" thickBot="1">
+      <c r="A97" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B96" s="21" t="s">
+      <c r="B97" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="C96" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D96" s="22" t="s">
+      <c r="C97" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D97" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="E96" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="20" t="s">
+      <c r="E97" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15" thickBot="1">
+      <c r="A98" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B97" s="21" t="s">
+      <c r="B98" s="21" t="s">
         <v>397</v>
       </c>
-      <c r="C97" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D97" s="22" t="s">
+      <c r="C98" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" s="22" t="s">
         <v>398</v>
       </c>
-      <c r="E97" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="20" t="s">
+      <c r="E98" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15" thickBot="1">
+      <c r="A99" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="B98" s="21" t="s">
+      <c r="B99" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="C98" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D98" s="22" t="s">
+      <c r="C99" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D99" s="22" t="s">
         <v>401</v>
       </c>
-      <c r="E98" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="20" t="s">
+      <c r="E99" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15" thickBot="1">
+      <c r="A100" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B100" s="21" t="s">
         <v>403</v>
       </c>
-      <c r="C99" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D99" s="22" t="s">
+      <c r="C100" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D100" s="22" t="s">
         <v>404</v>
       </c>
-      <c r="E99" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="20" t="s">
+      <c r="E100" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15" thickBot="1">
+      <c r="A101" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="B100" s="21" t="s">
+      <c r="B101" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="C100" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D100" s="22" t="s">
+      <c r="C101" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D101" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="E100" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="20" t="s">
+      <c r="E101" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A102" s="20" t="s">
         <v>408</v>
       </c>
-      <c r="B101" s="21" t="s">
+      <c r="B102" s="21" t="s">
         <v>409</v>
       </c>
-      <c r="C101" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D101" s="22" t="s">
+      <c r="C102" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D102" s="22" t="s">
         <v>410</v>
       </c>
-      <c r="E101" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="20" t="s">
+      <c r="E102" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A103" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="B102" s="21" t="s">
+      <c r="B103" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D102" s="22" t="s">
+      <c r="C103" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D103" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="E102" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="20" t="s">
+      <c r="E103" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A104" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B104" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="C103" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D103" s="22" t="s">
+      <c r="C104" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D104" s="22" t="s">
         <v>416</v>
       </c>
-      <c r="E103" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="20" t="s">
+      <c r="E104" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A105" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="B104" s="21" t="s">
+      <c r="B105" s="21" t="s">
         <v>418</v>
       </c>
-      <c r="C104" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D104" s="22" t="s">
+      <c r="C105" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D105" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="E104" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="20" t="s">
+      <c r="E105" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" thickBot="1">
+      <c r="A106" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="B106" s="21" t="s">
         <v>421</v>
       </c>
-      <c r="C105" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D105" s="22" t="s">
+      <c r="C106" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D106" s="22" t="s">
         <v>422</v>
       </c>
-      <c r="E105" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="20" t="s">
+      <c r="E106" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15" thickBot="1">
+      <c r="A107" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="B106" s="21" t="s">
+      <c r="B107" s="21" t="s">
         <v>424</v>
       </c>
-      <c r="C106" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D106" s="22" t="s">
+      <c r="C107" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D107" s="22" t="s">
         <v>425</v>
       </c>
-      <c r="E106" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="20" t="s">
+      <c r="E107" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15" thickBot="1">
+      <c r="A108" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="B107" s="21" t="s">
+      <c r="B108" s="21" t="s">
         <v>427</v>
       </c>
-      <c r="C107" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D107" s="22" t="s">
+      <c r="C108" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D108" s="22" t="s">
         <v>428</v>
       </c>
-      <c r="E107" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="20" t="s">
+      <c r="E108" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A109" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="B108" s="21" t="s">
+      <c r="B109" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="C108" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D108" s="22" t="s">
+      <c r="C109" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D109" s="22" t="s">
         <v>431</v>
       </c>
-      <c r="E108" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="20" t="s">
+      <c r="E109" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="26.5" thickBot="1">
+      <c r="A110" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B110" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="C109" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D109" s="22" t="s">
+      <c r="C110" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D110" s="22" t="s">
         <v>434</v>
       </c>
-      <c r="E109" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="20" t="s">
+      <c r="E110" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15" thickBot="1">
+      <c r="A111" s="20" t="s">
         <v>435</v>
       </c>
-      <c r="B110" s="21" t="s">
+      <c r="B111" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="C110" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D110" s="22" t="s">
+      <c r="C111" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D111" s="22" t="s">
         <v>437</v>
       </c>
-      <c r="E110" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="20" t="s">
+      <c r="E111" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15" thickBot="1">
+      <c r="A112" s="20" t="s">
         <v>438</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B112" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="C111" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D111" s="22" t="s">
+      <c r="C112" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D112" s="22" t="s">
         <v>440</v>
       </c>
-      <c r="E111" s="22" t="s">
+      <c r="E112" s="22" t="s">
         <v>441</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A112:XFD1048576 A58:B63 F2:XFD111">
+  <conditionalFormatting sqref="A1:XFD1 A113:XFD1048576 A59:B64 F2:XFD112">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update localization spreadsheet for end of round remove controls of ui from keyboard
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -448,9 +448,6 @@
     <t>Esperando a otros jugadores...</t>
   </si>
   <si>
-    <t>Partidas completadas</t>
-  </si>
-  <si>
     <t>Partida: {0}</t>
   </si>
   <si>
@@ -766,9 +763,6 @@
     <t>In attesa di altri giocatori</t>
   </si>
   <si>
-    <t>LIvelli completati</t>
-  </si>
-  <si>
     <t>Livello {0}</t>
   </si>
   <si>
@@ -1367,6 +1361,12 @@
   </si>
   <si>
     <t>Controles táctiles</t>
+  </si>
+  <si>
+    <t>LIvelli completati: {0}</t>
+  </si>
+  <si>
+    <t>Partidas completadas: {0}</t>
   </si>
 </sst>
 </file>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1961,13 +1961,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1">
@@ -1978,13 +1978,13 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1">
@@ -1995,13 +1995,13 @@
         <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1">
@@ -2012,13 +2012,13 @@
         <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1">
@@ -2029,13 +2029,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1">
@@ -2046,13 +2046,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>114</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1">
@@ -2063,13 +2063,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>115</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1">
@@ -2080,13 +2080,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1">
@@ -2097,13 +2097,13 @@
         <v>17</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>117</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1">
@@ -2114,13 +2114,13 @@
         <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1">
@@ -2131,13 +2131,13 @@
         <v>52</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1">
@@ -2148,13 +2148,13 @@
         <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>120</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1">
@@ -2165,30 +2165,30 @@
         <v>82</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1">
       <c r="A16" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>446</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1">
@@ -2199,13 +2199,13 @@
         <v>75</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>122</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1">
@@ -2216,13 +2216,13 @@
         <v>24</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>123</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1">
@@ -2233,13 +2233,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>124</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1">
@@ -2250,13 +2250,13 @@
         <v>89</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>125</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1">
@@ -2267,13 +2267,13 @@
         <v>90</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>126</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1">
@@ -2284,47 +2284,47 @@
         <v>26</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1">
       <c r="A23" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>204</v>
-      </c>
       <c r="C23" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1">
       <c r="A24" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>202</v>
-      </c>
       <c r="C24" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1">
@@ -2335,13 +2335,13 @@
         <v>27</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1">
@@ -2352,13 +2352,13 @@
         <v>28</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>129</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1">
@@ -2369,13 +2369,13 @@
         <v>31</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>130</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1">
@@ -2386,13 +2386,13 @@
         <v>36</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>131</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1">
@@ -2403,13 +2403,13 @@
         <v>37</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1">
@@ -2420,13 +2420,13 @@
         <v>38</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>133</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1">
@@ -2437,13 +2437,13 @@
         <v>39</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1">
@@ -2451,50 +2451,50 @@
         <v>40</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1">
       <c r="A33" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1">
@@ -2505,13 +2505,13 @@
         <v>54</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>135</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1">
@@ -2522,13 +2522,13 @@
         <v>56</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1">
@@ -2539,13 +2539,13 @@
         <v>60</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1">
@@ -2556,13 +2556,13 @@
         <v>59</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>136</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="23.5" thickBot="1">
@@ -2573,13 +2573,13 @@
         <v>62</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>137</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1">
@@ -2590,13 +2590,13 @@
         <v>69</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>138</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1">
@@ -2607,13 +2607,13 @@
         <v>70</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1">
@@ -2630,7 +2630,7 @@
         <v>140</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1">
@@ -2641,13 +2641,13 @@
         <v>74</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>141</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1">
@@ -2658,13 +2658,13 @@
         <v>78</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>142</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1">
@@ -2675,13 +2675,13 @@
         <v>84</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>143</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1">
@@ -2692,13 +2692,13 @@
         <v>29</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>250</v>
+        <v>449</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>144</v>
+        <v>450</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1">
@@ -2709,13 +2709,13 @@
         <v>71</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1">
@@ -2726,13 +2726,13 @@
         <v>72</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1">
@@ -2743,13 +2743,13 @@
         <v>80</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1">
@@ -2760,13 +2760,13 @@
         <v>86</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1">
@@ -2777,13 +2777,13 @@
         <v>92</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D51" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>192</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="23.5" thickBot="1">
@@ -2794,13 +2794,13 @@
         <v>94</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="23.5" thickBot="1">
@@ -2808,16 +2808,16 @@
         <v>96</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1">
@@ -2828,13 +2828,13 @@
         <v>100</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1">
@@ -2845,13 +2845,13 @@
         <v>103</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>104</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="35" thickBot="1">
@@ -2862,13 +2862,13 @@
         <v>106</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="23.5" thickBot="1">
@@ -2879,13 +2879,13 @@
         <v>97</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="46.5" thickBot="1">
@@ -2893,934 +2893,934 @@
         <v>108</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1">
       <c r="A59" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" thickBot="1">
       <c r="A60" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1">
       <c r="A61" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1">
       <c r="A62" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1">
       <c r="A63" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" thickBot="1">
       <c r="A64" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="D64" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="B64" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="D64" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>291</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" thickBot="1">
       <c r="A65" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="B65" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>299</v>
-      </c>
       <c r="E65" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="26.5" thickBot="1">
       <c r="A66" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D66" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="B66" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="C66" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D66" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="E66" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" thickBot="1">
       <c r="A67" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D67" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="B67" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>305</v>
-      </c>
       <c r="E67" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" thickBot="1">
       <c r="A68" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="B68" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>308</v>
-      </c>
       <c r="E68" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" thickBot="1">
       <c r="A69" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D69" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B69" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>311</v>
-      </c>
       <c r="E69" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="26.5" thickBot="1">
       <c r="A70" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D70" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="B70" s="21" t="s">
-        <v>313</v>
-      </c>
-      <c r="C70" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D70" s="23" t="s">
-        <v>314</v>
-      </c>
       <c r="E70" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" thickBot="1">
       <c r="A71" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D71" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="B71" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="C71" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D71" s="22" t="s">
-        <v>317</v>
-      </c>
       <c r="E71" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" thickBot="1">
       <c r="A72" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D72" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="B72" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>320</v>
-      </c>
       <c r="E72" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" thickBot="1">
       <c r="A73" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D73" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="B73" s="21" t="s">
-        <v>322</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>323</v>
-      </c>
       <c r="E73" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1">
       <c r="A74" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="B74" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>326</v>
-      </c>
       <c r="E74" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1">
       <c r="A75" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D75" s="22" t="s">
         <v>327</v>
       </c>
-      <c r="B75" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>329</v>
-      </c>
       <c r="E75" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1">
       <c r="A76" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D76" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="B76" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>332</v>
-      </c>
       <c r="E76" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1">
       <c r="A77" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="B77" s="21" t="s">
-        <v>334</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>335</v>
-      </c>
       <c r="E77" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" thickBot="1">
       <c r="A78" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D78" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="B78" s="21" t="s">
-        <v>337</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D78" s="22" t="s">
-        <v>338</v>
-      </c>
       <c r="E78" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1">
       <c r="A79" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="B79" s="21" t="s">
-        <v>340</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>341</v>
-      </c>
       <c r="E79" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1">
       <c r="A80" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D80" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="B80" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D80" s="22" t="s">
-        <v>344</v>
-      </c>
       <c r="E80" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1">
       <c r="A81" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="B81" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D81" s="22" t="s">
-        <v>347</v>
-      </c>
       <c r="E81" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1">
       <c r="A82" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D82" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="B82" s="21" t="s">
-        <v>349</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>350</v>
-      </c>
       <c r="E82" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1">
       <c r="A83" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>351</v>
       </c>
-      <c r="B83" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D83" s="22" t="s">
-        <v>353</v>
-      </c>
       <c r="E83" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1">
       <c r="A84" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D84" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="B84" s="21" t="s">
-        <v>355</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D84" s="22" t="s">
-        <v>356</v>
-      </c>
       <c r="E84" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" thickBot="1">
       <c r="A85" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="B85" s="21" t="s">
-        <v>358</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D85" s="22" t="s">
-        <v>359</v>
-      </c>
       <c r="E85" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" thickBot="1">
       <c r="A86" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D86" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="B86" s="21" t="s">
-        <v>361</v>
-      </c>
-      <c r="C86" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D86" s="22" t="s">
-        <v>362</v>
-      </c>
       <c r="E86" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" thickBot="1">
       <c r="A87" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="B87" s="21" t="s">
-        <v>364</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D87" s="22" t="s">
-        <v>365</v>
-      </c>
       <c r="E87" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" thickBot="1">
       <c r="A88" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D88" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="B88" s="21" t="s">
-        <v>367</v>
-      </c>
-      <c r="C88" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D88" s="22" t="s">
-        <v>368</v>
-      </c>
       <c r="E88" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" thickBot="1">
       <c r="A89" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D89" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="B89" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D89" s="22" t="s">
-        <v>371</v>
-      </c>
       <c r="E89" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15" thickBot="1">
       <c r="A90" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D90" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="B90" s="21" t="s">
-        <v>373</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D90" s="22" t="s">
-        <v>374</v>
-      </c>
       <c r="E90" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15" thickBot="1">
       <c r="A91" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="B91" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="C91" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D91" s="22" t="s">
-        <v>377</v>
-      </c>
       <c r="E91" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="26.5" thickBot="1">
       <c r="A92" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D92" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="B92" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="C92" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D92" s="22" t="s">
-        <v>380</v>
-      </c>
       <c r="E92" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1">
       <c r="A93" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D93" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="B93" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D93" s="22" t="s">
-        <v>383</v>
-      </c>
       <c r="E93" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1">
       <c r="A94" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D94" s="22" t="s">
         <v>384</v>
       </c>
-      <c r="B94" s="21" t="s">
-        <v>385</v>
-      </c>
-      <c r="C94" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D94" s="22" t="s">
-        <v>386</v>
-      </c>
       <c r="E94" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1">
       <c r="A95" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D95" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="B95" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="C95" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>389</v>
-      </c>
       <c r="E95" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1">
       <c r="A96" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>389</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D96" s="22" t="s">
         <v>390</v>
       </c>
-      <c r="B96" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>392</v>
-      </c>
       <c r="E96" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1">
       <c r="A97" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D97" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="B97" s="21" t="s">
-        <v>394</v>
-      </c>
-      <c r="C97" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D97" s="22" t="s">
-        <v>395</v>
-      </c>
       <c r="E97" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1">
       <c r="A98" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D98" s="22" t="s">
         <v>396</v>
       </c>
-      <c r="B98" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D98" s="22" t="s">
-        <v>398</v>
-      </c>
       <c r="E98" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1">
       <c r="A99" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D99" s="22" t="s">
         <v>399</v>
       </c>
-      <c r="B99" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D99" s="22" t="s">
-        <v>401</v>
-      </c>
       <c r="E99" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1">
       <c r="A100" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D100" s="22" t="s">
         <v>402</v>
       </c>
-      <c r="B100" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D100" s="22" t="s">
-        <v>404</v>
-      </c>
       <c r="E100" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1">
       <c r="A101" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D101" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="B101" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="C101" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D101" s="22" t="s">
-        <v>407</v>
-      </c>
       <c r="E101" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="26.5" thickBot="1">
       <c r="A102" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D102" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="B102" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="C102" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D102" s="22" t="s">
-        <v>410</v>
-      </c>
       <c r="E102" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="26.5" thickBot="1">
       <c r="A103" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D103" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="B103" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D103" s="22" t="s">
-        <v>413</v>
-      </c>
       <c r="E103" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="26.5" thickBot="1">
       <c r="A104" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D104" s="22" t="s">
         <v>414</v>
       </c>
-      <c r="B104" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D104" s="22" t="s">
-        <v>416</v>
-      </c>
       <c r="E104" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="26.5" thickBot="1">
       <c r="A105" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D105" s="22" t="s">
         <v>417</v>
       </c>
-      <c r="B105" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="C105" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>419</v>
-      </c>
       <c r="E105" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15" thickBot="1">
       <c r="A106" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D106" s="22" t="s">
         <v>420</v>
       </c>
-      <c r="B106" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="C106" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D106" s="22" t="s">
-        <v>422</v>
-      </c>
       <c r="E106" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15" thickBot="1">
       <c r="A107" s="20" t="s">
+        <v>421</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D107" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="B107" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D107" s="22" t="s">
-        <v>425</v>
-      </c>
       <c r="E107" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15" thickBot="1">
       <c r="A108" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D108" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="B108" s="21" t="s">
-        <v>427</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D108" s="22" t="s">
-        <v>428</v>
-      </c>
       <c r="E108" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="26.5" thickBot="1">
       <c r="A109" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>428</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D109" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="B109" s="21" t="s">
-        <v>430</v>
-      </c>
-      <c r="C109" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D109" s="22" t="s">
-        <v>431</v>
-      </c>
       <c r="E109" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="26.5" thickBot="1">
       <c r="A110" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D110" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="B110" s="21" t="s">
-        <v>433</v>
-      </c>
-      <c r="C110" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D110" s="22" t="s">
-        <v>434</v>
-      </c>
       <c r="E110" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15" thickBot="1">
       <c r="A111" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="C111" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D111" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="B111" s="21" t="s">
-        <v>436</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D111" s="22" t="s">
-        <v>437</v>
-      </c>
       <c r="E111" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15" thickBot="1">
       <c r="A112" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="C112" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="D112" s="22" t="s">
         <v>438</v>
       </c>
-      <c r="B112" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="C112" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="D112" s="22" t="s">
-        <v>440</v>
-      </c>
       <c r="E112" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update strings to include italian lesson descriptions
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/PP_LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="499">
   <si>
     <t>Key</t>
   </si>
@@ -1367,13 +1367,157 @@
   </si>
   <si>
     <t>Partidas completadas: {0}</t>
+  </si>
+  <si>
+    <t>sommare due numeri a una cifra a 18</t>
+  </si>
+  <si>
+    <t>sommare un numero ad una cifra ed un numero a due cifre fino a 19</t>
+  </si>
+  <si>
+    <t>sottrarre un numero ad una cifra a zero</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a due cifre a zero</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre numeri ad una cifra fino a 18</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre numeri ad una ed a due cifre a 20 incluso lo zero</t>
+  </si>
+  <si>
+    <t>sommare numeri a due cifre e unità</t>
+  </si>
+  <si>
+    <t>sommare numeri a due cifre e decine</t>
+  </si>
+  <si>
+    <t>sommare due numeri a due cifre</t>
+  </si>
+  <si>
+    <t>sommare tre numeri ad una cifra</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a due cifre e unità</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a due cifre e decine</t>
+  </si>
+  <si>
+    <t>sottrarre due numeri a due cifre a zero</t>
+  </si>
+  <si>
+    <t>sottrarre tre numeri ad una cifra a zero</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre tre numeri a due cifre</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 2 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 10 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 5 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>moltiplicare 2, 5, 10 con numeri a due cifre</t>
+  </si>
+  <si>
+    <t>sommare un numero a tre cifre e unità</t>
+  </si>
+  <si>
+    <t>sommare un numero a tre cifre e decine</t>
+  </si>
+  <si>
+    <t>sommare un numero a tre cifre e centinaia</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a tre cifre e unità</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a tre cifre e decine</t>
+  </si>
+  <si>
+    <t>sottrarre un numero a tre cifre e centinaia</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre un numero a tre cifre e unità</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre un numero a tre cifre e decine</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre un numero a tre cifre e centinaia</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 3 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 4 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>dividere per 10 e 100</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina dell'8 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre due numeri a tre cifre</t>
+  </si>
+  <si>
+    <t>sommare numeri a quattro cifre</t>
+  </si>
+  <si>
+    <t>sottrarre numeri a quattro cifre</t>
+  </si>
+  <si>
+    <t>sommare e sottrarre numeri a quattro cifre</t>
+  </si>
+  <si>
+    <t>moltiplicare la tabellina del 12 fino a 12 volte</t>
+  </si>
+  <si>
+    <t>moltiplicare numeri a due cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>moltiplicare numeri a tre cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>dividere un numero a due cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>dividere un numero a tre cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>moltiplicare numeri fino a quattro cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>riconoscere i quadrati dei numeri ed i simboli matematici</t>
+  </si>
+  <si>
+    <t>riconoscere i cubi dei numeri ed i simboli matematici</t>
+  </si>
+  <si>
+    <t>dividere numeri fino a quattro cifre per un numero ad una cifra</t>
+  </si>
+  <si>
+    <t>risolvere un'operazione (+,-,x, ÷) fino a numeri di quattro cifre</t>
+  </si>
+  <si>
+    <t>risolvere due operazioni fino a numeri di quattro cifre</t>
+  </si>
+  <si>
+    <t>risolvere tre operazioni fino a numeri di quattro cifre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1467,8 +1611,15 @@
       <color rgb="FF212121"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1485,6 +1636,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1512,10 +1668,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1586,8 +1743,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1905,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -3014,14 +3175,14 @@
       <c r="B65" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>439</v>
+      <c r="C65" s="15" t="s">
+        <v>451</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="E65" s="22" t="s">
-        <v>439</v>
+      <c r="E65" s="26" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="26.5" thickBot="1">
@@ -3031,14 +3192,14 @@
       <c r="B66" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="C66" s="22" t="s">
-        <v>439</v>
+      <c r="C66" s="15" t="s">
+        <v>452</v>
       </c>
       <c r="D66" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="E66" s="22" t="s">
-        <v>439</v>
+      <c r="E66" s="26" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" thickBot="1">
@@ -3048,14 +3209,14 @@
       <c r="B67" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C67" s="22" t="s">
-        <v>439</v>
+      <c r="C67" s="15" t="s">
+        <v>453</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="E67" s="22" t="s">
-        <v>439</v>
+      <c r="E67" s="26" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" thickBot="1">
@@ -3065,14 +3226,14 @@
       <c r="B68" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>439</v>
+      <c r="C68" s="15" t="s">
+        <v>454</v>
       </c>
       <c r="D68" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="E68" s="22" t="s">
-        <v>439</v>
+      <c r="E68" s="26" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" thickBot="1">
@@ -3082,31 +3243,31 @@
       <c r="B69" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>439</v>
+      <c r="C69" s="15" t="s">
+        <v>455</v>
       </c>
       <c r="D69" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="E69" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="26.5" thickBot="1">
+      <c r="E69" s="26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="29.5" thickBot="1">
       <c r="A70" s="20" t="s">
         <v>310</v>
       </c>
       <c r="B70" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>439</v>
+      <c r="C70" s="15" t="s">
+        <v>456</v>
       </c>
       <c r="D70" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="E70" s="22" t="s">
-        <v>439</v>
+      <c r="E70" s="26" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" thickBot="1">
@@ -3116,14 +3277,14 @@
       <c r="B71" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="C71" s="22" t="s">
-        <v>439</v>
+      <c r="C71" s="15" t="s">
+        <v>457</v>
       </c>
       <c r="D71" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="E71" s="22" t="s">
-        <v>439</v>
+      <c r="E71" s="26" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" thickBot="1">
@@ -3133,14 +3294,14 @@
       <c r="B72" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>439</v>
+      <c r="C72" s="15" t="s">
+        <v>458</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="E72" s="22" t="s">
-        <v>439</v>
+      <c r="E72" s="26" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" thickBot="1">
@@ -3150,14 +3311,14 @@
       <c r="B73" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="C73" s="22" t="s">
-        <v>439</v>
+      <c r="C73" s="15" t="s">
+        <v>459</v>
       </c>
       <c r="D73" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="E73" s="22" t="s">
-        <v>439</v>
+      <c r="E73" s="26" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1">
@@ -3167,14 +3328,14 @@
       <c r="B74" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="C74" s="22" t="s">
-        <v>439</v>
+      <c r="C74" s="15" t="s">
+        <v>460</v>
       </c>
       <c r="D74" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>439</v>
+      <c r="E74" s="26" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1">
@@ -3184,14 +3345,14 @@
       <c r="B75" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>439</v>
+      <c r="C75" s="15" t="s">
+        <v>461</v>
       </c>
       <c r="D75" s="22" t="s">
         <v>327</v>
       </c>
-      <c r="E75" s="22" t="s">
-        <v>439</v>
+      <c r="E75" s="26" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1">
@@ -3201,14 +3362,14 @@
       <c r="B76" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="C76" s="22" t="s">
-        <v>439</v>
+      <c r="C76" s="15" t="s">
+        <v>462</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="E76" s="22" t="s">
-        <v>439</v>
+      <c r="E76" s="26" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1">
@@ -3218,14 +3379,14 @@
       <c r="B77" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="22" t="s">
-        <v>439</v>
+      <c r="C77" s="15" t="s">
+        <v>463</v>
       </c>
       <c r="D77" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>439</v>
+      <c r="E77" s="26" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" thickBot="1">
@@ -3235,14 +3396,14 @@
       <c r="B78" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="C78" s="22" t="s">
-        <v>439</v>
+      <c r="C78" s="15" t="s">
+        <v>464</v>
       </c>
       <c r="D78" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="E78" s="22" t="s">
-        <v>439</v>
+      <c r="E78" s="26" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1">
@@ -3252,14 +3413,14 @@
       <c r="B79" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="C79" s="22" t="s">
-        <v>439</v>
+      <c r="C79" s="15" t="s">
+        <v>465</v>
       </c>
       <c r="D79" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>439</v>
+      <c r="E79" s="26" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1">
@@ -3269,14 +3430,14 @@
       <c r="B80" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="C80" s="22" t="s">
-        <v>439</v>
+      <c r="C80" s="15" t="s">
+        <v>466</v>
       </c>
       <c r="D80" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="E80" s="22" t="s">
-        <v>439</v>
+      <c r="E80" s="26" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1">
@@ -3286,14 +3447,14 @@
       <c r="B81" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="C81" s="22" t="s">
-        <v>439</v>
+      <c r="C81" s="15" t="s">
+        <v>467</v>
       </c>
       <c r="D81" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="E81" s="22" t="s">
-        <v>439</v>
+      <c r="E81" s="26" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1">
@@ -3303,14 +3464,14 @@
       <c r="B82" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="C82" s="22" t="s">
-        <v>439</v>
+      <c r="C82" s="15" t="s">
+        <v>468</v>
       </c>
       <c r="D82" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="E82" s="22" t="s">
-        <v>439</v>
+      <c r="E82" s="26" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1">
@@ -3320,14 +3481,14 @@
       <c r="B83" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="C83" s="22" t="s">
-        <v>439</v>
+      <c r="C83" s="15" t="s">
+        <v>469</v>
       </c>
       <c r="D83" s="22" t="s">
         <v>351</v>
       </c>
-      <c r="E83" s="22" t="s">
-        <v>439</v>
+      <c r="E83" s="26" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1">
@@ -3337,14 +3498,14 @@
       <c r="B84" s="21" t="s">
         <v>353</v>
       </c>
-      <c r="C84" s="22" t="s">
-        <v>439</v>
+      <c r="C84" s="15" t="s">
+        <v>470</v>
       </c>
       <c r="D84" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="E84" s="22" t="s">
-        <v>439</v>
+      <c r="E84" s="26" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" thickBot="1">
@@ -3354,14 +3515,14 @@
       <c r="B85" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="C85" s="22" t="s">
-        <v>439</v>
+      <c r="C85" s="15" t="s">
+        <v>471</v>
       </c>
       <c r="D85" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="E85" s="22" t="s">
-        <v>439</v>
+      <c r="E85" s="26" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" thickBot="1">
@@ -3371,14 +3532,14 @@
       <c r="B86" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="C86" s="22" t="s">
-        <v>439</v>
+      <c r="C86" s="15" t="s">
+        <v>472</v>
       </c>
       <c r="D86" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="E86" s="22" t="s">
-        <v>439</v>
+      <c r="E86" s="26" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" thickBot="1">
@@ -3388,14 +3549,14 @@
       <c r="B87" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="C87" s="22" t="s">
-        <v>439</v>
+      <c r="C87" s="15" t="s">
+        <v>473</v>
       </c>
       <c r="D87" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="E87" s="22" t="s">
-        <v>439</v>
+      <c r="E87" s="26" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" thickBot="1">
@@ -3405,14 +3566,14 @@
       <c r="B88" s="21" t="s">
         <v>365</v>
       </c>
-      <c r="C88" s="22" t="s">
-        <v>439</v>
+      <c r="C88" s="15" t="s">
+        <v>474</v>
       </c>
       <c r="D88" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="E88" s="22" t="s">
-        <v>439</v>
+      <c r="E88" s="26" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" thickBot="1">
@@ -3422,14 +3583,14 @@
       <c r="B89" s="21" t="s">
         <v>368</v>
       </c>
-      <c r="C89" s="22" t="s">
-        <v>439</v>
+      <c r="C89" s="15" t="s">
+        <v>475</v>
       </c>
       <c r="D89" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="E89" s="22" t="s">
-        <v>439</v>
+      <c r="E89" s="26" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15" thickBot="1">
@@ -3439,14 +3600,14 @@
       <c r="B90" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="C90" s="22" t="s">
-        <v>439</v>
+      <c r="C90" s="15" t="s">
+        <v>476</v>
       </c>
       <c r="D90" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="E90" s="22" t="s">
-        <v>439</v>
+      <c r="E90" s="26" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15" thickBot="1">
@@ -3456,31 +3617,31 @@
       <c r="B91" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="C91" s="22" t="s">
-        <v>439</v>
+      <c r="C91" s="15" t="s">
+        <v>477</v>
       </c>
       <c r="D91" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="E91" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="26.5" thickBot="1">
+      <c r="E91" s="26" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="29.5" thickBot="1">
       <c r="A92" s="20" t="s">
         <v>376</v>
       </c>
       <c r="B92" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="C92" s="22" t="s">
-        <v>439</v>
+      <c r="C92" s="15" t="s">
+        <v>478</v>
       </c>
       <c r="D92" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="E92" s="22" t="s">
-        <v>439</v>
+      <c r="E92" s="26" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1">
@@ -3490,14 +3651,14 @@
       <c r="B93" s="21" t="s">
         <v>380</v>
       </c>
-      <c r="C93" s="22" t="s">
-        <v>439</v>
+      <c r="C93" s="15" t="s">
+        <v>479</v>
       </c>
       <c r="D93" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="E93" s="22" t="s">
-        <v>439</v>
+      <c r="E93" s="26" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1">
@@ -3507,14 +3668,14 @@
       <c r="B94" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="C94" s="22" t="s">
-        <v>439</v>
+      <c r="C94" s="15" t="s">
+        <v>480</v>
       </c>
       <c r="D94" s="22" t="s">
         <v>384</v>
       </c>
-      <c r="E94" s="22" t="s">
-        <v>439</v>
+      <c r="E94" s="26" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1">
@@ -3524,14 +3685,14 @@
       <c r="B95" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="C95" s="22" t="s">
-        <v>439</v>
+      <c r="C95" s="15" t="s">
+        <v>481</v>
       </c>
       <c r="D95" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="E95" s="22" t="s">
-        <v>439</v>
+      <c r="E95" s="26" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1">
@@ -3541,14 +3702,14 @@
       <c r="B96" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="C96" s="22" t="s">
-        <v>439</v>
+      <c r="C96" s="15" t="s">
+        <v>482</v>
       </c>
       <c r="D96" s="22" t="s">
         <v>390</v>
       </c>
-      <c r="E96" s="22" t="s">
-        <v>439</v>
+      <c r="E96" s="26" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1">
@@ -3558,14 +3719,14 @@
       <c r="B97" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="C97" s="22" t="s">
-        <v>439</v>
+      <c r="C97" s="15" t="s">
+        <v>483</v>
       </c>
       <c r="D97" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="E97" s="22" t="s">
-        <v>439</v>
+      <c r="E97" s="26" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1">
@@ -3575,14 +3736,14 @@
       <c r="B98" s="21" t="s">
         <v>395</v>
       </c>
-      <c r="C98" s="22" t="s">
-        <v>439</v>
+      <c r="C98" s="15" t="s">
+        <v>484</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>396</v>
       </c>
-      <c r="E98" s="22" t="s">
-        <v>439</v>
+      <c r="E98" s="26" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1">
@@ -3592,14 +3753,14 @@
       <c r="B99" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="C99" s="22" t="s">
-        <v>439</v>
+      <c r="C99" s="15" t="s">
+        <v>485</v>
       </c>
       <c r="D99" s="22" t="s">
         <v>399</v>
       </c>
-      <c r="E99" s="22" t="s">
-        <v>439</v>
+      <c r="E99" s="26" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1">
@@ -3609,14 +3770,14 @@
       <c r="B100" s="21" t="s">
         <v>401</v>
       </c>
-      <c r="C100" s="22" t="s">
-        <v>439</v>
+      <c r="C100" s="15" t="s">
+        <v>486</v>
       </c>
       <c r="D100" s="22" t="s">
         <v>402</v>
       </c>
-      <c r="E100" s="22" t="s">
-        <v>439</v>
+      <c r="E100" s="26" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1">
@@ -3626,14 +3787,14 @@
       <c r="B101" s="21" t="s">
         <v>404</v>
       </c>
-      <c r="C101" s="22" t="s">
-        <v>439</v>
+      <c r="C101" s="15" t="s">
+        <v>487</v>
       </c>
       <c r="D101" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="E101" s="22" t="s">
-        <v>439</v>
+      <c r="E101" s="26" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="26.5" thickBot="1">
@@ -3643,14 +3804,14 @@
       <c r="B102" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>439</v>
+      <c r="C102" s="15" t="s">
+        <v>488</v>
       </c>
       <c r="D102" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="E102" s="22" t="s">
-        <v>439</v>
+      <c r="E102" s="26" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="26.5" thickBot="1">
@@ -3660,14 +3821,14 @@
       <c r="B103" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="C103" s="22" t="s">
-        <v>439</v>
+      <c r="C103" s="15" t="s">
+        <v>489</v>
       </c>
       <c r="D103" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="E103" s="22" t="s">
-        <v>439</v>
+      <c r="E103" s="26" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="26.5" thickBot="1">
@@ -3677,14 +3838,14 @@
       <c r="B104" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="C104" s="22" t="s">
-        <v>439</v>
+      <c r="C104" s="15" t="s">
+        <v>490</v>
       </c>
       <c r="D104" s="22" t="s">
         <v>414</v>
       </c>
-      <c r="E104" s="22" t="s">
-        <v>439</v>
+      <c r="E104" s="26" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="26.5" thickBot="1">
@@ -3694,48 +3855,48 @@
       <c r="B105" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="C105" s="22" t="s">
-        <v>439</v>
+      <c r="C105" s="15" t="s">
+        <v>491</v>
       </c>
       <c r="D105" s="22" t="s">
         <v>417</v>
       </c>
-      <c r="E105" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15" thickBot="1">
+      <c r="E105" s="26" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="26.5" thickBot="1">
       <c r="A106" s="20" t="s">
         <v>418</v>
       </c>
       <c r="B106" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="C106" s="22" t="s">
-        <v>439</v>
+      <c r="C106" s="15" t="s">
+        <v>492</v>
       </c>
       <c r="D106" s="22" t="s">
         <v>420</v>
       </c>
-      <c r="E106" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" thickBot="1">
+      <c r="E106" s="26" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="26.5" thickBot="1">
       <c r="A107" s="20" t="s">
         <v>421</v>
       </c>
       <c r="B107" s="21" t="s">
         <v>422</v>
       </c>
-      <c r="C107" s="22" t="s">
-        <v>439</v>
+      <c r="C107" s="15" t="s">
+        <v>493</v>
       </c>
       <c r="D107" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="E107" s="22" t="s">
-        <v>439</v>
+      <c r="E107" s="26" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15" thickBot="1">
@@ -3745,31 +3906,31 @@
       <c r="B108" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="C108" s="22" t="s">
-        <v>439</v>
+      <c r="C108" s="15" t="s">
+        <v>494</v>
       </c>
       <c r="D108" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="E108" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="26.5" thickBot="1">
+      <c r="E108" s="26" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="29.5" thickBot="1">
       <c r="A109" s="20" t="s">
         <v>427</v>
       </c>
       <c r="B109" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="C109" s="22" t="s">
-        <v>439</v>
+      <c r="C109" s="15" t="s">
+        <v>495</v>
       </c>
       <c r="D109" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="E109" s="22" t="s">
-        <v>439</v>
+      <c r="E109" s="26" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="26.5" thickBot="1">
@@ -3779,14 +3940,14 @@
       <c r="B110" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="C110" s="22" t="s">
-        <v>439</v>
+      <c r="C110" s="15" t="s">
+        <v>496</v>
       </c>
       <c r="D110" s="22" t="s">
         <v>432</v>
       </c>
-      <c r="E110" s="22" t="s">
-        <v>439</v>
+      <c r="E110" s="26" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15" thickBot="1">
@@ -3796,14 +3957,14 @@
       <c r="B111" s="21" t="s">
         <v>434</v>
       </c>
-      <c r="C111" s="22" t="s">
-        <v>439</v>
+      <c r="C111" s="15" t="s">
+        <v>497</v>
       </c>
       <c r="D111" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="E111" s="22" t="s">
-        <v>439</v>
+      <c r="E111" s="26" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15" thickBot="1">
@@ -3813,14 +3974,14 @@
       <c r="B112" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="C112" s="22" t="s">
-        <v>439</v>
+      <c r="C112" s="15" t="s">
+        <v>498</v>
       </c>
       <c r="D112" s="22" t="s">
         <v>438</v>
       </c>
-      <c r="E112" s="22" t="s">
-        <v>439</v>
+      <c r="E112" s="26" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>